<commit_message>
Mała aktualizacja! Dodano wybór heurystyk.
</commit_message>
<xml_diff>
--- a/baza_danych.xlsx
+++ b/baza_danych.xlsx
@@ -2126,16 +2126,16 @@
     <t>TYP</t>
   </si>
   <si>
+    <t>GÓRNY</t>
+  </si>
+  <si>
+    <t>LEWY</t>
+  </si>
+  <si>
+    <t>DOLNY</t>
+  </si>
+  <si>
     <t>PRAWY</t>
-  </si>
-  <si>
-    <t>DOLNY</t>
-  </si>
-  <si>
-    <t>LEWY</t>
-  </si>
-  <si>
-    <t>GÓRNY</t>
   </si>
   <si>
     <t>POLKA_ID</t>
@@ -21450,10 +21450,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>170005</v>
+        <v>70017</v>
       </c>
       <c r="B2">
-        <v>160015</v>
+        <v>50017</v>
       </c>
       <c r="C2" t="s">
         <v>702</v>
@@ -21461,76 +21461,76 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>40003</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>50005</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>40015</v>
+        <v>130030</v>
       </c>
       <c r="B4">
-        <v>50017</v>
+        <v>150027</v>
       </c>
       <c r="C4" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>120003</v>
+        <v>40003</v>
       </c>
       <c r="B5">
-        <v>130005</v>
+        <v>50005</v>
       </c>
       <c r="C5" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>120015</v>
+        <v>50017</v>
       </c>
       <c r="B6">
-        <v>160015</v>
+        <v>70017</v>
       </c>
       <c r="C6" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>80015</v>
+        <v>70027</v>
       </c>
       <c r="B7">
-        <v>120015</v>
+        <v>130030</v>
       </c>
       <c r="C7" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>100000</v>
+        <v>40015</v>
       </c>
       <c r="B8">
-        <v>140000</v>
+        <v>80015</v>
       </c>
       <c r="C8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>120003</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>140000</v>
+        <v>40015</v>
       </c>
       <c r="C9" t="s">
         <v>704</v>
@@ -21538,13 +21538,13 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>190005</v>
+        <v>150005</v>
       </c>
       <c r="B10">
-        <v>170005</v>
+        <v>130005</v>
       </c>
       <c r="C10" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -21552,18 +21552,18 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>40000</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>130017</v>
+        <v>170017</v>
       </c>
       <c r="B12">
-        <v>120017</v>
+        <v>150027</v>
       </c>
       <c r="C12" t="s">
         <v>705</v>
@@ -21571,54 +21571,54 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>40003</v>
+        <v>80015</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>40015</v>
       </c>
       <c r="C13" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>27</v>
+        <v>90017</v>
       </c>
       <c r="B14">
-        <v>10017</v>
+        <v>70027</v>
       </c>
       <c r="C14" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>110017</v>
+        <v>80003</v>
       </c>
       <c r="B15">
-        <v>90017</v>
+        <v>120003</v>
       </c>
       <c r="C15" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>27</v>
+        <v>120003</v>
       </c>
       <c r="B16">
-        <v>50027</v>
+        <v>160003</v>
       </c>
       <c r="C16" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>40003</v>
+        <v>170017</v>
       </c>
       <c r="B17">
-        <v>70000</v>
+        <v>190017</v>
       </c>
       <c r="C17" t="s">
         <v>704</v>
@@ -21626,32 +21626,32 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>30017</v>
+        <v>90005</v>
       </c>
       <c r="B18">
-        <v>10017</v>
+        <v>80005</v>
       </c>
       <c r="C18" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>140000</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>120003</v>
+        <v>10005</v>
       </c>
       <c r="C19" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>170005</v>
+        <v>5</v>
       </c>
       <c r="B20">
-        <v>160003</v>
+        <v>10005</v>
       </c>
       <c r="C20" t="s">
         <v>704</v>
@@ -21659,10 +21659,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>3</v>
+        <v>40005</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>50005</v>
       </c>
       <c r="C21" t="s">
         <v>704</v>
@@ -21670,76 +21670,76 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>10005</v>
+        <v>90017</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>110017</v>
       </c>
       <c r="C22" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>40000</v>
+        <v>70027</v>
       </c>
       <c r="B23">
-        <v>40003</v>
+        <v>130027</v>
       </c>
       <c r="C23" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>10005</v>
+        <v>40015</v>
       </c>
       <c r="B24">
-        <v>30005</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>3</v>
+        <v>10017</v>
       </c>
       <c r="B25">
-        <v>40003</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>170017</v>
+        <v>50017</v>
       </c>
       <c r="B26">
-        <v>160017</v>
+        <v>40015</v>
       </c>
       <c r="C26" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>120015</v>
+        <v>150027</v>
       </c>
       <c r="B27">
-        <v>130017</v>
+        <v>150031</v>
       </c>
       <c r="C27" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>50017</v>
+        <v>120003</v>
       </c>
       <c r="B28">
-        <v>50027</v>
+        <v>80003</v>
       </c>
       <c r="C28" t="s">
         <v>702</v>
@@ -21747,10 +21747,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>80015</v>
+        <v>80003</v>
       </c>
       <c r="B29">
-        <v>90017</v>
+        <v>40003</v>
       </c>
       <c r="C29" t="s">
         <v>702</v>
@@ -21758,10 +21758,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>130027</v>
+        <v>140000</v>
       </c>
       <c r="B30">
-        <v>70027</v>
+        <v>120003</v>
       </c>
       <c r="C30" t="s">
         <v>705</v>
@@ -21769,32 +21769,32 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>15</v>
+        <v>130005</v>
       </c>
       <c r="B31">
-        <v>10005</v>
+        <v>120003</v>
       </c>
       <c r="C31" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>190017</v>
+        <v>160015</v>
       </c>
       <c r="B32">
-        <v>170017</v>
+        <v>120015</v>
       </c>
       <c r="C32" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>100000</v>
+        <v>10005</v>
       </c>
       <c r="B33">
-        <v>70000</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
         <v>705</v>
@@ -21802,32 +21802,32 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
+        <v>70027</v>
+      </c>
+      <c r="B34">
         <v>50027</v>
       </c>
-      <c r="B34">
-        <v>27</v>
-      </c>
       <c r="C34" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>30005</v>
+        <v>120003</v>
       </c>
       <c r="B35">
-        <v>10005</v>
+        <v>140000</v>
       </c>
       <c r="C35" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>160017</v>
+        <v>80003</v>
       </c>
       <c r="B36">
-        <v>170017</v>
+        <v>100000</v>
       </c>
       <c r="C36" t="s">
         <v>703</v>
@@ -21835,98 +21835,98 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>50017</v>
+        <v>160003</v>
       </c>
       <c r="B37">
-        <v>40015</v>
+        <v>120003</v>
       </c>
       <c r="C37" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>90005</v>
+        <v>50017</v>
       </c>
       <c r="B38">
-        <v>80015</v>
+        <v>50027</v>
       </c>
       <c r="C38" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>50005</v>
+        <v>120003</v>
       </c>
       <c r="B39">
-        <v>40015</v>
+        <v>100000</v>
       </c>
       <c r="C39" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>90005</v>
+        <v>120015</v>
       </c>
       <c r="B40">
-        <v>110005</v>
+        <v>160015</v>
       </c>
       <c r="C40" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>50005</v>
+        <v>80015</v>
       </c>
       <c r="B41">
-        <v>70005</v>
+        <v>120015</v>
       </c>
       <c r="C41" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>120015</v>
+        <v>10017</v>
       </c>
       <c r="B42">
-        <v>80015</v>
+        <v>30017</v>
       </c>
       <c r="C42" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>130030</v>
+        <v>0</v>
       </c>
       <c r="B43">
-        <v>70027</v>
+        <v>40000</v>
       </c>
       <c r="C43" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>130005</v>
+        <v>170005</v>
       </c>
       <c r="B44">
-        <v>120003</v>
+        <v>160015</v>
       </c>
       <c r="C44" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>40003</v>
+        <v>170005</v>
       </c>
       <c r="B45">
-        <v>80003</v>
+        <v>160003</v>
       </c>
       <c r="C45" t="s">
         <v>703</v>
@@ -21934,43 +21934,43 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>40000</v>
+        <v>40015</v>
       </c>
       <c r="B46">
-        <v>70000</v>
+        <v>50017</v>
       </c>
       <c r="C46" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>170017</v>
+        <v>50005</v>
       </c>
       <c r="B47">
-        <v>160015</v>
+        <v>40015</v>
       </c>
       <c r="C47" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>160015</v>
+        <v>90005</v>
       </c>
       <c r="B48">
-        <v>170017</v>
+        <v>80015</v>
       </c>
       <c r="C48" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>10017</v>
+        <v>150027</v>
       </c>
       <c r="B49">
-        <v>27</v>
+        <v>130027</v>
       </c>
       <c r="C49" t="s">
         <v>702</v>
@@ -21978,87 +21978,87 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>80003</v>
+        <v>27</v>
       </c>
       <c r="B50">
-        <v>90005</v>
+        <v>50027</v>
       </c>
       <c r="C50" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>80003</v>
+        <v>120003</v>
       </c>
       <c r="B51">
-        <v>100000</v>
+        <v>130005</v>
       </c>
       <c r="C51" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>27</v>
+        <v>130017</v>
       </c>
       <c r="B52">
-        <v>31</v>
+        <v>120015</v>
       </c>
       <c r="C52" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>120003</v>
+        <v>160015</v>
       </c>
       <c r="B53">
-        <v>100000</v>
+        <v>170017</v>
       </c>
       <c r="C53" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>50027</v>
+        <v>10017</v>
       </c>
       <c r="B54">
-        <v>70027</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>110005</v>
+        <v>40003</v>
       </c>
       <c r="B55">
-        <v>90005</v>
+        <v>40000</v>
       </c>
       <c r="C55" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>70005</v>
+        <v>10017</v>
       </c>
       <c r="B56">
-        <v>50005</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>150031</v>
+        <v>10005</v>
       </c>
       <c r="B57">
-        <v>150027</v>
+        <v>30005</v>
       </c>
       <c r="C57" t="s">
         <v>704</v>
@@ -22066,54 +22066,54 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>80005</v>
+        <v>50005</v>
       </c>
       <c r="B58">
-        <v>90005</v>
+        <v>40005</v>
       </c>
       <c r="C58" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>50017</v>
+        <v>130005</v>
       </c>
       <c r="B59">
-        <v>40017</v>
+        <v>120005</v>
       </c>
       <c r="C59" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>160003</v>
+        <v>40000</v>
       </c>
       <c r="B60">
-        <v>170005</v>
+        <v>40003</v>
       </c>
       <c r="C60" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>150017</v>
+        <v>160017</v>
       </c>
       <c r="B61">
-        <v>130017</v>
+        <v>170017</v>
       </c>
       <c r="C61" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>17</v>
+        <v>170017</v>
       </c>
       <c r="B62">
-        <v>10017</v>
+        <v>160015</v>
       </c>
       <c r="C62" t="s">
         <v>703</v>
@@ -22121,43 +22121,43 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>130017</v>
+        <v>90017</v>
       </c>
       <c r="B63">
-        <v>120015</v>
+        <v>80015</v>
       </c>
       <c r="C63" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>140000</v>
+        <v>10005</v>
       </c>
       <c r="B64">
-        <v>100000</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>70000</v>
+        <v>90005</v>
       </c>
       <c r="B65">
-        <v>100000</v>
+        <v>110005</v>
       </c>
       <c r="C65" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>130027</v>
+        <v>50027</v>
       </c>
       <c r="B66">
-        <v>150027</v>
+        <v>50017</v>
       </c>
       <c r="C66" t="s">
         <v>703</v>
@@ -22165,10 +22165,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>40003</v>
+        <v>50005</v>
       </c>
       <c r="B67">
-        <v>40000</v>
+        <v>70005</v>
       </c>
       <c r="C67" t="s">
         <v>704</v>
@@ -22176,10 +22176,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>70000</v>
+        <v>120015</v>
       </c>
       <c r="B68">
-        <v>40000</v>
+        <v>130017</v>
       </c>
       <c r="C68" t="s">
         <v>705</v>
@@ -22187,87 +22187,87 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>10017</v>
+        <v>80015</v>
       </c>
       <c r="B69">
-        <v>15</v>
+        <v>90017</v>
       </c>
       <c r="C69" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>40000</v>
+        <v>40003</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>80003</v>
       </c>
       <c r="C70" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>10005</v>
+        <v>130030</v>
       </c>
       <c r="B71">
-        <v>5</v>
+        <v>130027</v>
       </c>
       <c r="C71" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>130017</v>
+        <v>40000</v>
       </c>
       <c r="B72">
-        <v>150017</v>
+        <v>70000</v>
       </c>
       <c r="C72" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>100000</v>
+        <v>150031</v>
       </c>
       <c r="B73">
-        <v>120003</v>
+        <v>150027</v>
       </c>
       <c r="C73" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>150027</v>
+        <v>100000</v>
       </c>
       <c r="B74">
-        <v>130030</v>
+        <v>140000</v>
       </c>
       <c r="C74" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>15</v>
+        <v>100000</v>
       </c>
       <c r="B75">
-        <v>10017</v>
+        <v>120003</v>
       </c>
       <c r="C75" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>100000</v>
+        <v>190005</v>
       </c>
       <c r="B76">
-        <v>80003</v>
+        <v>170005</v>
       </c>
       <c r="C76" t="s">
         <v>702</v>
@@ -22275,10 +22275,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>170005</v>
+        <v>100000</v>
       </c>
       <c r="B77">
-        <v>160005</v>
+        <v>80003</v>
       </c>
       <c r="C77" t="s">
         <v>705</v>
@@ -22286,98 +22286,98 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>70017</v>
+        <v>70027</v>
       </c>
       <c r="B78">
-        <v>50017</v>
+        <v>90017</v>
       </c>
       <c r="C78" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>80017</v>
+        <v>50027</v>
       </c>
       <c r="B79">
-        <v>90017</v>
+        <v>70027</v>
       </c>
       <c r="C79" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>40017</v>
+        <v>130017</v>
       </c>
       <c r="B80">
-        <v>50017</v>
+        <v>120017</v>
       </c>
       <c r="C80" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>150005</v>
+        <v>40003</v>
       </c>
       <c r="B81">
-        <v>130005</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>70027</v>
+        <v>80005</v>
       </c>
       <c r="B82">
-        <v>130030</v>
+        <v>90005</v>
       </c>
       <c r="C82" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>130005</v>
+        <v>50005</v>
       </c>
       <c r="B83">
-        <v>120015</v>
+        <v>40003</v>
       </c>
       <c r="C83" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>90017</v>
+        <v>90005</v>
       </c>
       <c r="B84">
-        <v>80015</v>
+        <v>80003</v>
       </c>
       <c r="C84" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>120005</v>
+        <v>110017</v>
       </c>
       <c r="B85">
-        <v>130005</v>
+        <v>90017</v>
       </c>
       <c r="C85" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
+        <v>80003</v>
+      </c>
+      <c r="B86">
         <v>90005</v>
-      </c>
-      <c r="B86">
-        <v>80005</v>
       </c>
       <c r="C86" t="s">
         <v>705</v>
@@ -22385,24 +22385,24 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>160005</v>
+        <v>30017</v>
       </c>
       <c r="B87">
-        <v>170005</v>
+        <v>10017</v>
       </c>
       <c r="C87" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>10005</v>
+        <v>27</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C88" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -22413,7 +22413,7 @@
         <v>160003</v>
       </c>
       <c r="C89" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -22424,37 +22424,37 @@
         <v>10005</v>
       </c>
       <c r="C90" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>50027</v>
+        <v>160015</v>
       </c>
       <c r="B91">
-        <v>50017</v>
+        <v>170005</v>
       </c>
       <c r="C91" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>130005</v>
+        <v>17</v>
       </c>
       <c r="B92">
-        <v>150005</v>
+        <v>10017</v>
       </c>
       <c r="C92" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>130030</v>
+        <v>3</v>
       </c>
       <c r="B93">
-        <v>130027</v>
+        <v>40003</v>
       </c>
       <c r="C93" t="s">
         <v>704</v>
@@ -22462,76 +22462,76 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>70000</v>
+        <v>31</v>
       </c>
       <c r="B94">
-        <v>80003</v>
+        <v>27</v>
       </c>
       <c r="C94" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>130027</v>
+        <v>70000</v>
       </c>
       <c r="B95">
-        <v>130030</v>
+        <v>100000</v>
       </c>
       <c r="C95" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>40015</v>
+        <v>130027</v>
       </c>
       <c r="B96">
-        <v>15</v>
+        <v>150027</v>
       </c>
       <c r="C96" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>120015</v>
+        <v>150027</v>
       </c>
       <c r="B97">
-        <v>130005</v>
+        <v>170017</v>
       </c>
       <c r="C97" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>80015</v>
+        <v>150017</v>
       </c>
       <c r="B98">
-        <v>90005</v>
+        <v>130017</v>
       </c>
       <c r="C98" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>10017</v>
+        <v>130017</v>
       </c>
       <c r="B99">
-        <v>17</v>
+        <v>150017</v>
       </c>
       <c r="C99" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>70000</v>
+        <v>170017</v>
       </c>
       <c r="B100">
-        <v>40003</v>
+        <v>160017</v>
       </c>
       <c r="C100" t="s">
         <v>702</v>
@@ -22542,40 +22542,40 @@
         <v>130027</v>
       </c>
       <c r="B101">
-        <v>130017</v>
+        <v>70027</v>
       </c>
       <c r="C101" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
-        <v>70027</v>
+        <v>190017</v>
       </c>
       <c r="B102">
-        <v>90017</v>
+        <v>170017</v>
       </c>
       <c r="C102" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103">
-        <v>80003</v>
+        <v>100000</v>
       </c>
       <c r="B103">
-        <v>40003</v>
+        <v>70000</v>
       </c>
       <c r="C103" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104">
-        <v>120003</v>
+        <v>160003</v>
       </c>
       <c r="B104">
-        <v>80003</v>
+        <v>170005</v>
       </c>
       <c r="C104" t="s">
         <v>705</v>
@@ -22583,43 +22583,43 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105">
-        <v>160015</v>
+        <v>50027</v>
       </c>
       <c r="B105">
-        <v>120015</v>
+        <v>27</v>
       </c>
       <c r="C105" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106">
-        <v>80003</v>
+        <v>30005</v>
       </c>
       <c r="B106">
-        <v>70000</v>
+        <v>10005</v>
       </c>
       <c r="C106" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107">
-        <v>70027</v>
+        <v>80017</v>
       </c>
       <c r="B107">
-        <v>50027</v>
+        <v>90017</v>
       </c>
       <c r="C107" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108">
-        <v>90005</v>
+        <v>40017</v>
       </c>
       <c r="B108">
-        <v>80003</v>
+        <v>50017</v>
       </c>
       <c r="C108" t="s">
         <v>704</v>
@@ -22627,76 +22627,76 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109">
-        <v>50005</v>
+        <v>120015</v>
       </c>
       <c r="B109">
-        <v>40003</v>
+        <v>80015</v>
       </c>
       <c r="C109" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110">
-        <v>170005</v>
+        <v>130030</v>
       </c>
       <c r="B110">
-        <v>190005</v>
+        <v>70027</v>
       </c>
       <c r="C110" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111">
-        <v>160003</v>
+        <v>120015</v>
       </c>
       <c r="B111">
-        <v>120003</v>
+        <v>130005</v>
       </c>
       <c r="C111" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112">
-        <v>160015</v>
+        <v>80015</v>
       </c>
       <c r="B112">
-        <v>170005</v>
+        <v>90005</v>
       </c>
       <c r="C112" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113">
-        <v>120017</v>
+        <v>120005</v>
       </c>
       <c r="B113">
-        <v>130017</v>
+        <v>130005</v>
       </c>
       <c r="C113" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114">
-        <v>0</v>
+        <v>160005</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>170005</v>
       </c>
       <c r="C114" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115">
-        <v>90017</v>
+        <v>15</v>
       </c>
       <c r="B115">
-        <v>80017</v>
+        <v>10017</v>
       </c>
       <c r="C115" t="s">
         <v>705</v>
@@ -22704,46 +22704,46 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116">
-        <v>170017</v>
+        <v>130005</v>
       </c>
       <c r="B116">
-        <v>150027</v>
+        <v>150005</v>
       </c>
       <c r="C116" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117">
-        <v>31</v>
+        <v>40015</v>
       </c>
       <c r="B117">
-        <v>27</v>
+        <v>50005</v>
       </c>
       <c r="C117" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118">
-        <v>150027</v>
+        <v>130027</v>
       </c>
       <c r="B118">
-        <v>170017</v>
+        <v>130017</v>
       </c>
       <c r="C118" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119">
-        <v>90017</v>
+        <v>70031</v>
       </c>
       <c r="B119">
         <v>70027</v>
       </c>
       <c r="C119" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -22754,15 +22754,15 @@
         <v>70031</v>
       </c>
       <c r="C120" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121">
-        <v>10017</v>
+        <v>80003</v>
       </c>
       <c r="B121">
-        <v>30017</v>
+        <v>70000</v>
       </c>
       <c r="C121" t="s">
         <v>703</v>
@@ -22770,43 +22770,43 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122">
-        <v>150027</v>
+        <v>160003</v>
       </c>
       <c r="B122">
-        <v>130027</v>
+        <v>140000</v>
       </c>
       <c r="C122" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123">
-        <v>130030</v>
+        <v>110005</v>
       </c>
       <c r="B123">
-        <v>150027</v>
+        <v>90005</v>
       </c>
       <c r="C123" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124">
-        <v>50017</v>
+        <v>70005</v>
       </c>
       <c r="B124">
-        <v>70017</v>
+        <v>50005</v>
       </c>
       <c r="C124" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125">
-        <v>80015</v>
+        <v>130005</v>
       </c>
       <c r="B125">
-        <v>40015</v>
+        <v>120015</v>
       </c>
       <c r="C125" t="s">
         <v>705</v>
@@ -22814,32 +22814,32 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126">
-        <v>40015</v>
+        <v>130017</v>
       </c>
       <c r="B126">
-        <v>80015</v>
+        <v>130027</v>
       </c>
       <c r="C126" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127">
-        <v>15</v>
+        <v>170005</v>
       </c>
       <c r="B127">
-        <v>40015</v>
+        <v>190005</v>
       </c>
       <c r="C127" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128">
-        <v>130017</v>
+        <v>50017</v>
       </c>
       <c r="B128">
-        <v>130027</v>
+        <v>40017</v>
       </c>
       <c r="C128" t="s">
         <v>702</v>
@@ -22847,43 +22847,43 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129">
-        <v>150027</v>
+        <v>70000</v>
       </c>
       <c r="B129">
-        <v>150031</v>
+        <v>80003</v>
       </c>
       <c r="C129" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130">
-        <v>120003</v>
+        <v>130027</v>
       </c>
       <c r="B130">
-        <v>160003</v>
+        <v>130030</v>
       </c>
       <c r="C130" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131">
-        <v>80003</v>
+        <v>140000</v>
       </c>
       <c r="B131">
-        <v>120003</v>
+        <v>100000</v>
       </c>
       <c r="C131" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132">
-        <v>50005</v>
+        <v>70000</v>
       </c>
       <c r="B132">
-        <v>40005</v>
+        <v>40003</v>
       </c>
       <c r="C132" t="s">
         <v>705</v>
@@ -22891,101 +22891,101 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133">
-        <v>170017</v>
+        <v>120017</v>
       </c>
       <c r="B133">
-        <v>190017</v>
+        <v>130017</v>
       </c>
       <c r="C133" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134">
-        <v>40005</v>
+        <v>70000</v>
       </c>
       <c r="B134">
-        <v>50005</v>
+        <v>40000</v>
       </c>
       <c r="C134" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135">
-        <v>5</v>
+        <v>40000</v>
       </c>
       <c r="B135">
-        <v>10005</v>
+        <v>0</v>
       </c>
       <c r="C135" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136">
-        <v>90017</v>
+        <v>10005</v>
       </c>
       <c r="B136">
-        <v>110017</v>
+        <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137">
-        <v>70027</v>
+        <v>150027</v>
       </c>
       <c r="B137">
-        <v>130027</v>
+        <v>130030</v>
       </c>
       <c r="C137" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138">
-        <v>130005</v>
+        <v>27</v>
       </c>
       <c r="B138">
-        <v>120005</v>
+        <v>10017</v>
       </c>
       <c r="C138" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139">
-        <v>40015</v>
+        <v>90017</v>
       </c>
       <c r="B139">
-        <v>50005</v>
+        <v>80017</v>
       </c>
       <c r="C139" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140">
-        <v>70031</v>
+        <v>40003</v>
       </c>
       <c r="B140">
-        <v>70027</v>
+        <v>70000</v>
       </c>
       <c r="C140" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141">
-        <v>160003</v>
+        <v>170005</v>
       </c>
       <c r="B141">
-        <v>140000</v>
+        <v>160005</v>
       </c>
       <c r="C141" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>